<commit_message>
Configured BFF and added commons library
</commit_message>
<xml_diff>
--- a/files/database/User.xlsx
+++ b/files/database/User.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Username</t>
   </si>
@@ -83,6 +83,21 @@
   </si>
   <si>
     <t>vladpassword</t>
+  </si>
+  <si>
+    <t>elvis</t>
+  </si>
+  <si>
+    <t>Presly</t>
+  </si>
+  <si>
+    <t>Elviaso</t>
+  </si>
+  <si>
+    <t>ep@yahoo.com</t>
+  </si>
+  <si>
+    <t>elvispassword</t>
   </si>
 </sst>
 </file>
@@ -90,9 +105,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -142,20 +157,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -164,26 +165,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -192,6 +185,21 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -203,6 +211,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -211,7 +242,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -219,32 +250,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -257,37 +272,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -299,25 +380,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,115 +446,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,17 +481,46 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -499,35 +543,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -535,16 +550,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -553,142 +568,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1030,13 +1045,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="15.7777777777778" customWidth="1"/>
     <col min="4" max="4" width="29.2222222222222" customWidth="1"/>
@@ -1134,8 +1149,31 @@
       <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1143,6 +1181,7 @@
     <hyperlink ref="D3" r:id="rId1" display="alexandruolteanu2001@gmail.com"/>
     <hyperlink ref="D4" r:id="rId2" display="andreeapotcovaru21@yahoo.com"/>
     <hyperlink ref="D5" r:id="rId3" display="vd@yahoo.com"/>
+    <hyperlink ref="D6" r:id="rId4" display="ep@yahoo.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>